<commit_message>
se modificó titulo a la sección LTL
</commit_message>
<xml_diff>
--- a/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
+++ b/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_hub_LogisLJC\migracion\05-Portal_Interno\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\migracion\05-Portal_Interno\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CE1AA6-6674-4B88-80D3-C595A3EEB5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B45C478-3172-41ED-B0B0-810F8097600F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="138">
   <si>
     <t>Comercio exterior</t>
   </si>
@@ -436,9 +436,6 @@
   </si>
   <si>
     <t>Cancelaci&amp;oacute;n masiva de talones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTL solo cambia el titulo </t>
   </si>
   <si>
     <t>Distribucion</t>
@@ -987,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E15CABE-9918-48E5-AC3B-82373F41E1D6}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1001,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -1031,7 +1028,7 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1058,7 +1055,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>48</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
@@ -1085,7 +1082,7 @@
       </c>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>49</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>51</v>
@@ -1130,7 +1127,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1148,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1169,7 @@
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1190,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1214,7 +1211,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1232,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1253,7 @@
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1267,7 +1264,7 @@
         <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>57</v>
@@ -1318,7 +1315,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>123</v>
       </c>
@@ -1355,7 +1352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1372,7 +1369,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1389,7 +1386,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>67</v>
       </c>
@@ -1403,10 +1400,10 @@
         <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>68</v>
       </c>
@@ -1417,13 +1414,13 @@
         <v>36</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>69</v>
       </c>
@@ -1437,7 +1434,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>71</v>
       </c>
@@ -1462,7 +1459,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>72</v>
       </c>
@@ -1473,7 +1470,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>73</v>
       </c>
@@ -1484,7 +1481,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>74</v>
       </c>
@@ -1495,7 +1492,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>75</v>
       </c>
@@ -1506,7 +1503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>76</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>77</v>
       </c>
@@ -1528,7 +1525,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>78</v>
       </c>
@@ -1539,7 +1536,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>7</v>
       </c>
@@ -1550,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>79</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1571,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>81</v>
       </c>
@@ -1590,7 +1587,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>78</v>
       </c>
@@ -1598,7 +1595,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1606,7 +1603,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>8</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>79</v>
       </c>
@@ -1622,7 +1619,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
         <v>7</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>8</v>
       </c>
@@ -1638,7 +1635,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B45" s="6" t="s">
         <v>82</v>
       </c>
@@ -1646,7 +1643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
         <v>81</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1662,7 +1659,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
         <v>7</v>
       </c>
@@ -1670,7 +1667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
         <v>8</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
         <v>79</v>
       </c>
@@ -1686,7 +1683,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
         <v>7</v>
       </c>
@@ -1694,7 +1691,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
         <v>8</v>
       </c>
@@ -1702,7 +1699,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>77</v>
       </c>
@@ -1710,7 +1707,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>78</v>
       </c>
@@ -1718,7 +1715,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B55" s="9" t="s">
         <v>7</v>
       </c>
@@ -1726,7 +1723,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B56" s="9" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1731,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>79</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B58" s="9" t="s">
         <v>7</v>
       </c>
@@ -1750,7 +1747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B59" s="9" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D60" s="7" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
Se actualizó el archivo excel
</commit_message>
<xml_diff>
--- a/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
+++ b/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\migracion\05-Portal_Interno\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B45C478-3172-41ED-B0B0-810F8097600F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83667C29-507D-4536-B018-4467B072DE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="140">
   <si>
     <t>Comercio exterior</t>
   </si>
@@ -432,12 +432,6 @@
     <t>Work Arround</t>
   </si>
   <si>
-    <t>Cancelar tal&amp;oacute;n</t>
-  </si>
-  <si>
-    <t>Cancelaci&amp;oacute;n masiva de talones</t>
-  </si>
-  <si>
     <t>Distribucion</t>
   </si>
   <si>
@@ -448,6 +442,18 @@
   </si>
   <si>
     <t>Reservar guias</t>
+  </si>
+  <si>
+    <t>Cancelar talón</t>
+  </si>
+  <si>
+    <t>Cancelación masiva de talones</t>
+  </si>
+  <si>
+    <t>ltl_disponibles(dentro del módulo)</t>
+  </si>
+  <si>
+    <t>cd_disponibles(dentro del módulo)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -569,6 +575,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E15CABE-9918-48E5-AC3B-82373F41E1D6}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +1006,7 @@
     <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.140625" bestFit="1" customWidth="1"/>
@@ -1050,7 +1062,7 @@
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="11" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="8"/>
@@ -1072,12 +1084,12 @@
         <v>48</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="11" t="s">
         <v>125</v>
       </c>
       <c r="I5" s="8"/>
@@ -1096,17 +1108,17 @@
         <v>49</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="11" t="s">
         <v>117</v>
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1122,8 +1134,8 @@
       <c r="F7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>128</v>
+      <c r="H7" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="I7" s="8"/>
     </row>
@@ -1143,8 +1155,8 @@
       <c r="F8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>126</v>
+      <c r="H8" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="I8" s="8"/>
     </row>
@@ -1164,8 +1176,8 @@
       <c r="F9" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>116</v>
+      <c r="H9" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="I9" s="8"/>
     </row>
@@ -1185,8 +1197,8 @@
       <c r="F10" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>129</v>
+      <c r="H10" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="I10" s="8"/>
     </row>
@@ -1206,8 +1218,8 @@
       <c r="F11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>130</v>
+      <c r="H11" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="I11" s="8"/>
     </row>
@@ -1227,8 +1239,8 @@
       <c r="F12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>119</v>
+      <c r="H12" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="I12" s="8"/>
     </row>
@@ -1248,8 +1260,8 @@
       <c r="F13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>128</v>
+      <c r="H13" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="I13" s="8"/>
     </row>
@@ -1269,12 +1281,12 @@
       <c r="F14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>131</v>
+      <c r="H14" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
@@ -1290,12 +1302,12 @@
       <c r="F15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>132</v>
+      <c r="H15" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1311,8 +1323,8 @@
       <c r="F16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>133</v>
+      <c r="H16" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
@@ -1331,8 +1343,8 @@
       <c r="F17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>118</v>
+      <c r="H17" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
@@ -1351,6 +1363,9 @@
       <c r="F18" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="H18" s="11" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -1368,6 +1383,9 @@
       <c r="F19" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="H19" s="11" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
@@ -1385,6 +1403,9 @@
       <c r="F20" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="H20" s="11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
@@ -1400,8 +1421,9 @@
         <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>137</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
@@ -1414,7 +1436,7 @@
         <v>36</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>128</v>
@@ -1433,6 +1455,9 @@
       <c r="E23" s="6" t="s">
         <v>113</v>
       </c>
+      <c r="F23" s="11" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
@@ -1446,6 +1471,9 @@
       </c>
       <c r="E24" s="7" t="s">
         <v>114</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Se actualiza listado de módulos del portal interno
</commit_message>
<xml_diff>
--- a/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
+++ b/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\migracion\05-Portal_Interno\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion\05-Portal_Interno\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83667C29-507D-4536-B018-4467B072DE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEB8063-CA35-4158-B342-5D0F285950BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -450,10 +448,10 @@
     <t>Cancelación masiva de talones</t>
   </si>
   <si>
-    <t>ltl_disponibles(dentro del módulo)</t>
-  </si>
-  <si>
-    <t>cd_disponibles(dentro del módulo)</t>
+    <t>Ltl</t>
+  </si>
+  <si>
+    <t>CrossDock</t>
   </si>
 </sst>
 </file>
@@ -628,7 +626,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12953932" cy="1114286"/>
+          <a:ext cx="12953372" cy="1114286"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="11692550" cy="1114286"/>
         </a:xfrm>
@@ -996,9 +994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E15CABE-9918-48E5-AC3B-82373F41E1D6}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1013,7 +1009,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -1040,8 +1036,8 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1067,8 +1063,8 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1094,7 +1090,7 @@
       </c>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1114,7 @@
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1139,7 +1135,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1160,7 +1156,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1177,7 @@
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1202,7 +1198,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1223,7 +1219,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1240,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1265,7 +1261,7 @@
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1327,7 +1323,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1347,7 +1343,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>123</v>
       </c>
@@ -1367,7 +1363,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1387,7 +1383,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1425,7 +1421,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>68</v>
       </c>
@@ -1442,7 +1438,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>69</v>
       </c>
@@ -1459,7 +1455,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
@@ -1472,7 +1468,7 @@
       <c r="E24" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1553,7 +1549,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>78</v>
       </c>
@@ -1564,7 +1560,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
         <v>7</v>
       </c>
@@ -1575,7 +1571,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>8</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>79</v>
       </c>
@@ -1591,7 +1587,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1599,7 +1595,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1607,7 +1603,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>81</v>
       </c>
@@ -1615,7 +1611,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>78</v>
       </c>
@@ -1623,7 +1619,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>8</v>
       </c>
@@ -1639,7 +1635,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>7</v>
       </c>
@@ -1655,7 +1651,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>8</v>
       </c>
@@ -1663,7 +1659,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>82</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>81</v>
       </c>
@@ -1679,7 +1675,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1687,7 +1683,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>8</v>
       </c>
@@ -1703,7 +1699,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>79</v>
       </c>
@@ -1711,7 +1707,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1715,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>8</v>
       </c>
@@ -1727,7 +1723,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
         <v>77</v>
       </c>
@@ -1735,7 +1731,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>78</v>
       </c>
@@ -1743,7 +1739,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>7</v>
       </c>
@@ -1751,7 +1747,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>8</v>
       </c>
@@ -1759,7 +1755,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>79</v>
       </c>
@@ -1767,7 +1763,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1771,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
         <v>8</v>
       </c>
@@ -1783,7 +1779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
se quitan sangrias que se tenian de mas
</commit_message>
<xml_diff>
--- a/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
+++ b/05-Portal_Interno/00-Documentacion/Modulos_Porta-Internol-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion\05-Portal_Interno\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEB8063-CA35-4158-B342-5D0F285950BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E9B17E-798B-47F1-B0BE-7C18A1A4F9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -994,7 +994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E15CABE-9918-48E5-AC3B-82373F41E1D6}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1468,11 +1470,11 @@
       <c r="E24" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>71</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>72</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>73</v>
       </c>
@@ -1505,7 +1507,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>74</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>75</v>
       </c>
@@ -1527,7 +1529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>76</v>
       </c>
@@ -1538,7 +1540,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>77</v>
       </c>

</xml_diff>